<commit_message>
validate that text file contains zoom chat pattern
</commit_message>
<xml_diff>
--- a/server/test/files_to_test/students_list_excel/example_excel.xlsx
+++ b/server/test/files_to_test/students_list_excel/example_excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Inbar Shirizly\Documents\python\useful\ITC_programs\zoom_attendance_check\student_csv_examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Inbar Shirizly\Documents\python\useful\ITC_programs\zoom_attendance_check\server\test\files_to_test\students_list_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB068EB0-396B-4828-B121-3902584F36BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D19B91-93F7-476C-B459-C23425556D96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{488C6C20-8654-4E36-919F-D3E2AD714F5E}"/>
+    <workbookView xWindow="2364" yWindow="3684" windowWidth="17280" windowHeight="8976" xr2:uid="{488C6C20-8654-4E36-919F-D3E2AD714F5E}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -434,13 +434,14 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="21.21875" customWidth="1"/>
     <col min="9" max="10" width="15.33203125" customWidth="1"/>
     <col min="11" max="11" width="13.33203125" customWidth="1"/>
   </cols>

</xml_diff>